<commit_message>
Improving layout adding columns and result expander
</commit_message>
<xml_diff>
--- a/bjj_videos.xlsx
+++ b/bjj_videos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berku\Desktop\DSI\Personal Git Hub\Bjj Videos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berku\Desktop\DSI\Personal Git Hub\bjj_video_encyclopedia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FFC088A-90A7-4627-AD4C-8B26A7B38DAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4220E10-8EDE-46FB-9547-4F0C2567C9EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{105A8B3C-B0DF-4E11-A285-0EF1E8A311BD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="98">
   <si>
     <t>Link</t>
   </si>
@@ -238,13 +238,103 @@
   </si>
   <si>
     <t>00:02:40</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ojvH99btFYo&amp;ab_channel=BernardoFariaBJJFanatics</t>
+  </si>
+  <si>
+    <t>Leonardo Nogueira</t>
+  </si>
+  <si>
+    <t>Half Guard</t>
+  </si>
+  <si>
+    <t>00:01:22</t>
+  </si>
+  <si>
+    <t>Basic principles of the half gard, with knee shield</t>
+  </si>
+  <si>
+    <t>00:08:28</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=usFjw23WsMI&amp;ab_channel=GRACIEMAG</t>
+  </si>
+  <si>
+    <t>Carlson Gracie Jr</t>
+  </si>
+  <si>
+    <t>00:01:07</t>
+  </si>
+  <si>
+    <t>00:02:19</t>
+  </si>
+  <si>
+    <t>Passing</t>
+  </si>
+  <si>
+    <t>Spider Guard</t>
+  </si>
+  <si>
+    <t>Finalização Relogio</t>
+  </si>
+  <si>
+    <t>00:01:30</t>
+  </si>
+  <si>
+    <t>Turtle</t>
+  </si>
+  <si>
+    <t>sweep</t>
+  </si>
+  <si>
+    <t>Arm lock variation.</t>
+  </si>
+  <si>
+    <t>00:02:35</t>
+  </si>
+  <si>
+    <t>Opponent is on the side of the turtle</t>
+  </si>
+  <si>
+    <t>Opponent is on front of the turtle</t>
+  </si>
+  <si>
+    <t>00:02:54</t>
+  </si>
+  <si>
+    <t>00:04:50</t>
+  </si>
+  <si>
+    <t>North South</t>
+  </si>
+  <si>
+    <t>00:06:30</t>
+  </si>
+  <si>
+    <t>Sparring</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=lYGLz0sagH8&amp;ab_channel=GracieBarra</t>
+  </si>
+  <si>
+    <t>Marcio Feitosa &amp; Marcelo Souza</t>
+  </si>
+  <si>
+    <t>00:05:00</t>
+  </si>
+  <si>
+    <t>00:05:31</t>
+  </si>
+  <si>
+    <t>Open Guard,</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,6 +346,14 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -278,15 +376,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -599,10 +700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38FAC974-A4D0-46B2-849E-EA9FC55454A3}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -997,7 +1098,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B14" t="s">
@@ -1026,9 +1127,176 @@
       <c r="A15" t="s">
         <v>34</v>
       </c>
-      <c r="I15" s="1"/>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" t="s">
+        <v>82</v>
+      </c>
+      <c r="F15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" t="s">
+        <v>83</v>
+      </c>
+      <c r="H15" t="s">
+        <v>84</v>
+      </c>
+      <c r="I15" t="s">
+        <v>86</v>
+      </c>
+      <c r="J15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E16" t="s">
+        <v>82</v>
+      </c>
+      <c r="F16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" t="s">
+        <v>83</v>
+      </c>
+      <c r="H16" t="s">
+        <v>84</v>
+      </c>
+      <c r="I16" t="s">
+        <v>87</v>
+      </c>
+      <c r="J16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E17" t="s">
+        <v>82</v>
+      </c>
+      <c r="F17" t="s">
+        <v>90</v>
+      </c>
+      <c r="G17" t="s">
+        <v>83</v>
+      </c>
+      <c r="I17" s="1"/>
+      <c r="J17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" t="s">
+        <v>33</v>
+      </c>
+      <c r="I18" t="s">
+        <v>72</v>
+      </c>
+      <c r="J18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" t="s">
+        <v>79</v>
+      </c>
+      <c r="F19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" t="s">
+        <v>78</v>
+      </c>
+      <c r="H19" t="s">
+        <v>80</v>
+      </c>
+      <c r="J19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" t="s">
+        <v>94</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G20" t="s">
+        <v>92</v>
+      </c>
+      <c r="I20" t="s">
+        <v>97</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A18" r:id="rId1" xr:uid="{F531A8DE-71B4-4F67-B8C4-2809733FE7EB}"/>
+    <hyperlink ref="A19" r:id="rId2" xr:uid="{B3BB94DF-BD68-431F-AAF7-68FF198AA0AB}"/>
+  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>